<commit_message>
Bar graph is added!
</commit_message>
<xml_diff>
--- a/Overestimation_scenarios.xlsx
+++ b/Overestimation_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebyG\Documents\GitHub\Zeo-CO2-H2S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F51844E4-F60F-4A95-996F-D18FD71508A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF7D420-074E-4015-A735-4ACAEE49ED4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{ED159BDA-2D36-4193-A6EC-9AA7179B301F}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{ED159BDA-2D36-4193-A6EC-9AA7179B301F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>200% overestimated</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>CDO_1 (CO2)</t>
+  </si>
+  <si>
+    <t>0% overestimated</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB79C22C-22E6-4044-87B3-A91C64CAF5A0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,61 +453,81 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>0.68237641507562896</v>
+        <v>0.55405849026174403</v>
       </c>
       <c r="C2">
-        <v>0.81275027033320402</v>
+        <v>0.621582133488505</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>0.776060279602515</v>
+        <v>0.69596385110244496</v>
       </c>
       <c r="G2">
-        <v>0.76357742357935998</v>
+        <v>0.53694284724367503</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.78463482028850995</v>
+        <v>0.68237641507562896</v>
       </c>
       <c r="C3">
-        <v>0.89322704511868001</v>
+        <v>0.81275027033320402</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>0.82049296693215001</v>
+        <v>0.776060279602515</v>
       </c>
       <c r="G3">
-        <v>0.86263620801844398</v>
+        <v>0.76357742357935998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.78463482028850995</v>
+      </c>
+      <c r="C4">
+        <v>0.89322704511868001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.82049296693215001</v>
+      </c>
+      <c r="G4">
+        <v>0.86263620801844398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.88535878012307301</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.95862690699465802</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>0.89248922066816305</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>0.94375337817259697</v>
       </c>
     </row>

</xml_diff>